<commit_message>
Update analysis of first and second experiments.
</commit_message>
<xml_diff>
--- a/Biocontrole.xlsx
+++ b/Biocontrole.xlsx
@@ -198,12 +198,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -225,6 +226,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -343,7 +352,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -367,13 +376,31 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -381,7 +408,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,7 +416,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,75 +424,75 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,34 +512,40 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="12">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Pivot Table Corner" xfId="20"/>
+    <cellStyle name="Pivot Table Value" xfId="21"/>
+    <cellStyle name="Pivot Table Field" xfId="22"/>
+    <cellStyle name="Pivot Table Category" xfId="23"/>
+    <cellStyle name="Pivot Table Title" xfId="24"/>
+    <cellStyle name="Pivot Table Result" xfId="25"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -588,14 +621,12 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="7" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -751,7 +782,7 @@
       </c>
       <c r="D6" s="12" t="n">
         <f aca="false">STDEV(B6:B8)</f>
-        <v>1.28582010146572</v>
+        <v>1.28582010146573</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="17" t="s">
@@ -929,7 +960,7 @@
       </c>
       <c r="D12" s="22" t="n">
         <f aca="false">STDEV(B12:B14)</f>
-        <v>0.702376916856851</v>
+        <v>0.702376916856849</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="13" t="s">
@@ -1427,7 +1458,7 @@
       </c>
       <c r="D33" s="22" t="n">
         <f aca="false">STDEV(B33:B35)</f>
-        <v>1.04083299973306</v>
+        <v>1.04083299973307</v>
       </c>
       <c r="E33" s="25"/>
     </row>
@@ -1532,7 +1563,7 @@
       </c>
       <c r="D42" s="22" t="n">
         <f aca="false">STDEV(B42:B44)</f>
-        <v>1.7616280348965</v>
+        <v>1.76162803489651</v>
       </c>
       <c r="E42" s="25"/>
     </row>
@@ -1666,7 +1697,7 @@
       </c>
       <c r="D54" s="22" t="n">
         <f aca="false">STDEV(B54:B56)</f>
-        <v>1.16761865920914</v>
+        <v>1.16761865920913</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1921,7 @@
       </c>
       <c r="D75" s="22" t="n">
         <f aca="false">STDEV(B75:B77)</f>
-        <v>0.896288643983255</v>
+        <v>0.89628864398325</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2081,7 @@
       </c>
       <c r="D90" s="22" t="n">
         <f aca="false">STDEV(B90:B92)</f>
-        <v>0.550757054728611</v>
+        <v>0.55075705472861</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,7 +2113,7 @@
       </c>
       <c r="D93" s="22" t="n">
         <f aca="false">STDEV(B93:B95)</f>
-        <v>0.832666399786463</v>
+        <v>0.832666399786453</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,7 +2337,7 @@
       </c>
       <c r="D114" s="22" t="n">
         <f aca="false">STDEV(B114:B116)</f>
-        <v>0.814452781524713</v>
+        <v>0.814452781524708</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2402,7 +2433,7 @@
       </c>
       <c r="D123" s="28" t="n">
         <f aca="false">STDEV(B123:B125)</f>
-        <v>0.929157324317755</v>
+        <v>0.929157324317757</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,15 +2766,15 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="10.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="5.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="30" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="4.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="7.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="30" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>